<commit_message>
Task Utilisation updated based upon the latest code
</commit_message>
<xml_diff>
--- a/30_Software/Embed/Task_Utilisation.xlsx
+++ b/30_Software/Embed/Task_Utilisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_Projects\02_Hephaestus\miStepper\30_Software\Embed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7392313D-014A-44FE-8A25-7D19B595F76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE2500F-A239-407A-B1C2-6EA2A410963B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF01F588-D711-4D40-97CC-7BE325704FCE}"/>
+    <workbookView xWindow="28680" yWindow="-13620" windowWidth="24240" windowHeight="13140" xr2:uid="{BF01F588-D711-4D40-97CC-7BE325704FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisation" sheetId="1" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>160 B / 504 B</t>
   </si>
   <si>
-    <t>0x2cd6 (1.1%)</t>
-  </si>
-  <si>
     <t>0x20001c08</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>0x20002290</t>
   </si>
   <si>
-    <t>0x17819 (9.0%)</t>
-  </si>
-  <si>
     <t>0x20001e88</t>
   </si>
   <si>
@@ -208,27 +202,15 @@
     <t>0x20002908</t>
   </si>
   <si>
-    <t>416 B / 1.48 kB</t>
-  </si>
-  <si>
-    <t>0x1000 (0.4%)</t>
-  </si>
-  <si>
     <t>0x20002308</t>
   </si>
   <si>
     <t>0x200028f8</t>
   </si>
   <si>
-    <t>0x20002758</t>
-  </si>
-  <si>
     <t>0x20002d88</t>
   </si>
   <si>
-    <t>0xd03d (5.0%)</t>
-  </si>
-  <si>
     <t>0x20002980</t>
   </si>
   <si>
@@ -244,9 +226,6 @@
     <t>384 B / 504 B</t>
   </si>
   <si>
-    <t>0xa78c (4.0%)</t>
-  </si>
-  <si>
     <t>0x20002e00</t>
   </si>
   <si>
@@ -259,9 +238,6 @@
     <t>304 B / 504 B</t>
   </si>
   <si>
-    <t>0xa (0.0%)</t>
-  </si>
-  <si>
     <t>0x20003080</t>
   </si>
   <si>
@@ -277,9 +253,6 @@
     <t>336 B / 504 B</t>
   </si>
   <si>
-    <t>0x401 (0.1%)</t>
-  </si>
-  <si>
     <t>0x20003300</t>
   </si>
   <si>
@@ -301,9 +274,6 @@
     <t>764 B / 1.49 kB</t>
   </si>
   <si>
-    <t>0x20c (0.0%)</t>
-  </si>
-  <si>
     <t>0x20003580</t>
   </si>
   <si>
@@ -316,19 +286,49 @@
     <t>0x20003d08</t>
   </si>
   <si>
-    <t>80 B / 248 B</t>
-  </si>
-  <si>
-    <t>0xd0998 (80.3%)</t>
-  </si>
-  <si>
     <t>0x20003c00</t>
   </si>
   <si>
     <t>0x20003cf8</t>
   </si>
   <si>
-    <t>0x20003ca8</t>
+    <t>0x3122 (1.9%)</t>
+  </si>
+  <si>
+    <t>0xe86f (9.2%)</t>
+  </si>
+  <si>
+    <t>452 B / 1.48 kB</t>
+  </si>
+  <si>
+    <t>0x4ed2 (3.1%)</t>
+  </si>
+  <si>
+    <t>0x20002734</t>
+  </si>
+  <si>
+    <t>0x7963 (4.8%)</t>
+  </si>
+  <si>
+    <t>0x680a (4.1%)</t>
+  </si>
+  <si>
+    <t>0xf (0.0%)</t>
+  </si>
+  <si>
+    <t>0x96a (0.4%)</t>
+  </si>
+  <si>
+    <t>0x112 (0.0%)</t>
+  </si>
+  <si>
+    <t>88 B / 248 B</t>
+  </si>
+  <si>
+    <t>0x78702 (76.4%)</t>
+  </si>
+  <si>
+    <t>0x20003ca0</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
   <dimension ref="A1:AM46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" ref="J2:J8" si="0">MATCH(W2, $A:$A, 0)</f>
@@ -1031,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20002758</v>
+        <v>0x20002734</v>
       </c>
       <c r="N4" s="3" t="str">
         <f t="shared" si="9"/>
@@ -1059,19 +1059,19 @@
       </c>
       <c r="P4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002758</v>
+        <v>20002734</v>
       </c>
       <c r="Q4" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>416/1.48k</v>
+        <v>452/1.48k</v>
       </c>
       <c r="R4" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="S4" s="4">
         <f>INT(_xlfn.IFNA(LEFT(R4,LEN(R4)-1)*CHOOSE(MATCH(RIGHT(R4,1), {"K","M","B"},0),1000,1000000,1000000000),R4))</f>
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="T4" s="3" t="str">
         <f t="shared" si="2"/>
@@ -1095,11 +1095,11 @@
       </c>
       <c r="Z4" s="5">
         <f t="shared" si="15"/>
-        <v>1104</v>
+        <v>1068</v>
       </c>
       <c r="AA4" s="6">
         <f t="shared" si="16"/>
-        <v>0.72631578947368425</v>
+        <v>0.70263157894736838</v>
       </c>
       <c r="AB4" s="7">
         <f t="shared" si="17"/>
@@ -1107,11 +1107,11 @@
       </c>
       <c r="AC4" s="7">
         <f t="shared" si="18"/>
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="AD4" s="6">
         <f t="shared" si="19"/>
-        <v>0.2810810810810811</v>
+        <v>0.30540540540540539</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
@@ -1207,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
@@ -1298,7 +1298,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1310,7 +1310,7 @@
         <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="0"/>
@@ -1486,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" ref="J9:J35" si="20">MATCH(W9, $A:$A, 0)</f>
@@ -1574,7 +1574,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="20"/>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="M10" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20003ca8</v>
+        <v>0x20003ca0</v>
       </c>
       <c r="N10" s="3" t="str">
         <f t="shared" si="21"/>
@@ -1602,19 +1602,19 @@
       </c>
       <c r="P10" s="3" t="str">
         <f t="shared" si="23"/>
-        <v>20003ca8</v>
+        <v>20003ca0</v>
       </c>
       <c r="Q10" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>80/248</v>
+        <v>88/248</v>
       </c>
       <c r="R10" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="S10" s="5">
         <f>INT(_xlfn.IFNA(LEFT(R10,LEN(R10)-1)*CHOOSE(MATCH(RIGHT(R10,1), {"K","M","B"},0),1000,1000000,1000000000),R10))</f>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="T10" s="3" t="str">
         <f t="shared" si="25"/>
@@ -1638,11 +1638,11 @@
       </c>
       <c r="Z10" s="5">
         <f>IFERROR(HEX2DEC(P10)-HEX2DEC(N10), "")</f>
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="AA10" s="6">
         <f>IFERROR(Z10/Y10, "")</f>
-        <v>0.67741935483870963</v>
+        <v>0.64516129032258063</v>
       </c>
       <c r="AB10" s="7">
         <f>IFERROR(U10, "")</f>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="AC10" s="7">
         <f>IFERROR(S10, "")</f>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="AD10" s="6">
         <f>IFERROR(AC10/AB10, "")</f>
-        <v>0.32258064516129031</v>
+        <v>0.35483870967741937</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J11" s="5" t="e">
         <f t="shared" si="20"/>
@@ -1753,7 +1753,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
@@ -1762,10 +1762,10 @@
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="J12" s="5" t="e">
         <f t="shared" si="20"/>
@@ -1941,7 +1941,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J14" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2029,7 +2029,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J15" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2117,7 +2117,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="J16" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2208,7 +2208,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -2220,7 +2220,7 @@
         <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="J17" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2396,7 +2396,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J19" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2484,7 +2484,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J20" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2572,7 +2572,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J21" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2663,7 +2663,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -2672,10 +2672,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="J22" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2851,7 +2851,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="J24" s="5" t="e">
         <f t="shared" si="20"/>
@@ -2939,7 +2939,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J25" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3118,7 +3118,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -3127,10 +3127,10 @@
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="J27" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3306,7 +3306,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="J29" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3394,7 +3394,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="J30" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3482,7 +3482,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J31" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3573,7 +3573,7 @@
         <v>44</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -3582,10 +3582,10 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="J32" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3761,7 +3761,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J34" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3849,7 +3849,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J35" s="5" t="e">
         <f t="shared" si="20"/>
@@ -3937,7 +3937,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -3945,22 +3945,22 @@
         <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
@@ -3976,7 +3976,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -3984,7 +3984,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
@@ -3992,7 +3992,7 @@
         <v>15</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
@@ -4003,7 +4003,7 @@
         <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>1</v>
@@ -4012,10 +4012,10 @@
         <v>26</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
@@ -4031,7 +4031,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
@@ -4039,7 +4039,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Utilisation updated to show how the size of I2C has been consumed with the introduction of the BME280 controller
</commit_message>
<xml_diff>
--- a/30_Software/Embed/Task_Utilisation.xlsx
+++ b/30_Software/Embed/Task_Utilisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_Projects\02_Hephaestus\miStepper\30_Software\Embed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA889978-8D16-4CA1-8288-C38A499AFCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CF024B-1964-44DE-B08A-12C72BD3DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-13620" windowWidth="24240" windowHeight="13140" xr2:uid="{BF01F588-D711-4D40-97CC-7BE325704FCE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF01F588-D711-4D40-97CC-7BE325704FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Utilisation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>defaultTask</t>
   </si>
@@ -169,100 +169,13 @@
     <t>384 B / 504 B</t>
   </si>
   <si>
-    <t>0x20003080</t>
-  </si>
-  <si>
-    <t>336 B / 504 B</t>
-  </si>
-  <si>
-    <t>0x20003300</t>
-  </si>
-  <si>
-    <t>0x20002118</t>
-  </si>
-  <si>
-    <t>0x20001f10</t>
-  </si>
-  <si>
-    <t>0x20002108</t>
-  </si>
-  <si>
-    <t>0x20002598</t>
-  </si>
-  <si>
-    <t>0x20002190</t>
-  </si>
-  <si>
-    <t>0x20002588</t>
-  </si>
-  <si>
-    <t>0x20002348</t>
-  </si>
-  <si>
-    <t>0x20002c10</t>
-  </si>
-  <si>
-    <t>0x20002610</t>
-  </si>
-  <si>
-    <t>0x20002c00</t>
-  </si>
-  <si>
-    <t>0x20003090</t>
-  </si>
-  <si>
-    <t>0x20002c88</t>
-  </si>
-  <si>
-    <t>0x20002e40</t>
-  </si>
-  <si>
-    <t>0x20003310</t>
-  </si>
-  <si>
-    <t>0x20003108</t>
-  </si>
-  <si>
-    <t>0x20003180</t>
-  </si>
-  <si>
     <t>MotorManager</t>
-  </si>
-  <si>
-    <t>0x20003388</t>
   </si>
   <si>
     <t>Snapshot Water Mark (Words)</t>
   </si>
   <si>
-    <t>144 B / 504 B</t>
-  </si>
-  <si>
-    <t>0x24ba (3.1%)</t>
-  </si>
-  <si>
-    <t>0x20002078</t>
-  </si>
-  <si>
-    <t>0x6cfc (9.1%)</t>
-  </si>
-  <si>
     <t>580 B / 1.48 kB</t>
-  </si>
-  <si>
-    <t>0x1801 (2.0%)</t>
-  </si>
-  <si>
-    <t>0x200029bc</t>
-  </si>
-  <si>
-    <t>0x3033 (4.0%)</t>
-  </si>
-  <si>
-    <t>0x3b94 (4.9%)</t>
-  </si>
-  <si>
-    <t>0x20003590</t>
   </si>
   <si>
     <t>296 B / 504 B</t>
@@ -271,43 +184,133 @@
     <t>0x2 (0.0%)</t>
   </si>
   <si>
-    <t>0x20003580</t>
-  </si>
-  <si>
-    <t>0x20003458</t>
-  </si>
-  <si>
-    <t>0x20003810</t>
-  </si>
-  <si>
-    <t>0xc1d (1.0%)</t>
-  </si>
-  <si>
-    <t>0x20003608</t>
-  </si>
-  <si>
-    <t>0x20003800</t>
-  </si>
-  <si>
-    <t>0x200036b0</t>
-  </si>
-  <si>
-    <t>0x20003990</t>
-  </si>
-  <si>
     <t>88 B / 248 B</t>
   </si>
   <si>
-    <t>0x39261 (75.9%)</t>
+    <t>0x20002150</t>
   </si>
   <si>
-    <t>0x20003888</t>
+    <t>120 B / 504 B</t>
   </si>
   <si>
-    <t>0x20003980</t>
+    <t>0x1 (0.0%)</t>
   </si>
   <si>
-    <t>0x20003928</t>
+    <t>0x20001f48</t>
+  </si>
+  <si>
+    <t>0x20002140</t>
+  </si>
+  <si>
+    <t>0x200020c8</t>
+  </si>
+  <si>
+    <t>0x200025d0</t>
+  </si>
+  <si>
+    <t>0x33db (9.1%)</t>
+  </si>
+  <si>
+    <t>0x200021c8</t>
+  </si>
+  <si>
+    <t>0x200025c0</t>
+  </si>
+  <si>
+    <t>0x20002380</t>
+  </si>
+  <si>
+    <t>0x20002c48</t>
+  </si>
+  <si>
+    <t>0x5bc (1.0%)</t>
+  </si>
+  <si>
+    <t>0x20002648</t>
+  </si>
+  <si>
+    <t>0x20002c38</t>
+  </si>
+  <si>
+    <t>0x200029f4</t>
+  </si>
+  <si>
+    <t>0x200030c8</t>
+  </si>
+  <si>
+    <t>840 B / 1016 B</t>
+  </si>
+  <si>
+    <t>0x2264 (6.0%)</t>
+  </si>
+  <si>
+    <t>0x20002cc0</t>
+  </si>
+  <si>
+    <t>0x200030b8</t>
+  </si>
+  <si>
+    <t>0x20002d70</t>
+  </si>
+  <si>
+    <t>0x20003348</t>
+  </si>
+  <si>
+    <t>0x1ca4 (5.0%)</t>
+  </si>
+  <si>
+    <t>0x20003140</t>
+  </si>
+  <si>
+    <t>0x20003338</t>
+  </si>
+  <si>
+    <t>0x200031b8</t>
+  </si>
+  <si>
+    <t>0x200035c8</t>
+  </si>
+  <si>
+    <t>304 B / 504 B</t>
+  </si>
+  <si>
+    <t>0x200033c0</t>
+  </si>
+  <si>
+    <t>0x200035b8</t>
+  </si>
+  <si>
+    <t>0x20003488</t>
+  </si>
+  <si>
+    <t>0x20003848</t>
+  </si>
+  <si>
+    <t>0x5ba (1.0%)</t>
+  </si>
+  <si>
+    <t>0x20003640</t>
+  </si>
+  <si>
+    <t>0x20003838</t>
+  </si>
+  <si>
+    <t>0x20003710</t>
+  </si>
+  <si>
+    <t>0x200039c8</t>
+  </si>
+  <si>
+    <t>0x1be66 (77.9%)</t>
+  </si>
+  <si>
+    <t>0x200038c0</t>
+  </si>
+  <si>
+    <t>0x200039b8</t>
+  </si>
+  <si>
+    <t>0x20003960</t>
   </si>
 </sst>
 </file>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1C121E-8E6B-43F2-B7E5-7D463A544849}">
   <dimension ref="A1:AN200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -816,7 +819,7 @@
         <v>38</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>36</v>
@@ -830,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -839,10 +842,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" ref="J2:J8" si="0">MATCH(W2, $A:$A, 0)</f>
@@ -850,39 +853,39 @@
       </c>
       <c r="K2" s="3" t="str">
         <f>INDEX($A:$H, $J2+2, 3)</f>
-        <v>0x20001f10</v>
+        <v>0x20001f48</v>
       </c>
       <c r="L2" s="3" t="str">
         <f>INDEX($A:$H, $J2+3, 3)</f>
-        <v>0x20002108</v>
+        <v>0x20002140</v>
       </c>
       <c r="M2" s="3" t="str">
         <f>INDEX($A:$H, $J2+4, 3)</f>
-        <v>0x20002078</v>
+        <v>0x200020c8</v>
       </c>
       <c r="N2" s="3" t="str">
         <f>RIGHT(K2,LEN(K2)-2)</f>
-        <v>20001f10</v>
+        <v>20001f48</v>
       </c>
       <c r="O2" s="3" t="str">
         <f t="shared" ref="O2:P8" si="1">RIGHT(L2,LEN(L2)-2)</f>
-        <v>20002108</v>
+        <v>20002140</v>
       </c>
       <c r="P2" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002078</v>
+        <v>200020c8</v>
       </c>
       <c r="Q2" s="3" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(INDEX($A:$H, $J2, 6), " ", ""), "B", "")</f>
-        <v>144/504</v>
+        <v>120/504</v>
       </c>
       <c r="R2" s="3" t="str">
         <f>MID(Q2, 1, FIND("/", Q2, 1)-1)</f>
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="S2" s="4">
         <f>INT(_xlfn.IFNA(LEFT(R2,LEN(R2)-1)*CHOOSE(MATCH(RIGHT(R2,1), {"K","M","B"},0),1000,1000000,1000000000),R2))</f>
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="T2" s="3" t="str">
         <f t="shared" ref="T2:T8" si="2">MID(Q2,FIND("/",Q2,1)+1,LEN(Q2))</f>
@@ -905,11 +908,11 @@
       </c>
       <c r="Z2" s="4">
         <f t="shared" ref="Z2" si="5">HEX2DEC(P2)-HEX2DEC(N2)</f>
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="AA2" s="6">
         <f>Z2/Y2</f>
-        <v>0.7142857142857143</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="AB2" s="7">
         <f>U2</f>
@@ -917,15 +920,15 @@
       </c>
       <c r="AC2" s="7">
         <f>S2</f>
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="AD2" s="7">
         <f>IFERROR(AC2/4, "")</f>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="AE2" s="6">
         <f>AC2/AB2</f>
-        <v>0.2857142857142857</v>
+        <v>0.23809523809523808</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -941,27 +944,27 @@
       </c>
       <c r="K3" s="3" t="str">
         <f t="shared" ref="K3:K66" si="6">INDEX($A:$H, $J3+2, 3)</f>
-        <v>0x20002190</v>
+        <v>0x200021c8</v>
       </c>
       <c r="L3" s="3" t="str">
         <f t="shared" ref="L3:L66" si="7">INDEX($A:$H, $J3+3, 3)</f>
-        <v>0x20002588</v>
+        <v>0x200025c0</v>
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" ref="M3:M66" si="8">INDEX($A:$H, $J3+4, 3)</f>
-        <v>0x20002348</v>
+        <v>0x20002380</v>
       </c>
       <c r="N3" s="3" t="str">
         <f t="shared" ref="N3:N8" si="9">RIGHT(K3,LEN(K3)-2)</f>
-        <v>20002190</v>
+        <v>200021c8</v>
       </c>
       <c r="O3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002588</v>
+        <v>200025c0</v>
       </c>
       <c r="P3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002348</v>
+        <v>20002380</v>
       </c>
       <c r="Q3" s="3" t="str">
         <f t="shared" ref="Q3:Q66" si="10">SUBSTITUTE(SUBSTITUTE(INDEX($A:$H, $J3, 6), " ", ""), "B", "")</f>
@@ -1025,7 +1028,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="0"/>
@@ -1033,27 +1036,27 @@
       </c>
       <c r="K4" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20002610</v>
+        <v>0x20002648</v>
       </c>
       <c r="L4" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20002c00</v>
+        <v>0x20002c38</v>
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x200029bc</v>
+        <v>0x200029f4</v>
       </c>
       <c r="N4" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20002610</v>
+        <v>20002648</v>
       </c>
       <c r="O4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002c00</v>
+        <v>20002c38</v>
       </c>
       <c r="P4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>200029bc</v>
+        <v>200029f4</v>
       </c>
       <c r="Q4" s="3" t="str">
         <f t="shared" si="10"/>
@@ -1117,7 +1120,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="0"/>
@@ -1125,39 +1128,39 @@
       </c>
       <c r="K5" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20002c88</v>
+        <v>0x20002cc0</v>
       </c>
       <c r="L5" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20003080</v>
+        <v>0x200030b8</v>
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20002e40</v>
+        <v>0x20002d70</v>
       </c>
       <c r="N5" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20002c88</v>
+        <v>20002cc0</v>
       </c>
       <c r="O5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003080</v>
+        <v>200030b8</v>
       </c>
       <c r="P5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20002e40</v>
+        <v>20002d70</v>
       </c>
       <c r="Q5" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>576/1016</v>
+        <v>840/1016</v>
       </c>
       <c r="R5" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>576</v>
+        <v>840</v>
       </c>
       <c r="S5" s="4">
         <f>INT(_xlfn.IFNA(LEFT(R5,LEN(R5)-1)*CHOOSE(MATCH(RIGHT(R5,1), {"K","M","B"},0),1000,1000000,1000000000),R5))</f>
-        <v>576</v>
+        <v>840</v>
       </c>
       <c r="T5" s="3" t="str">
         <f t="shared" si="2"/>
@@ -1181,11 +1184,11 @@
       </c>
       <c r="Z5" s="5">
         <f t="shared" si="15"/>
-        <v>440</v>
+        <v>176</v>
       </c>
       <c r="AA5" s="6">
         <f t="shared" si="16"/>
-        <v>0.43307086614173229</v>
+        <v>0.17322834645669291</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="17"/>
@@ -1193,15 +1196,15 @@
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="18"/>
-        <v>576</v>
+        <v>840</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="19"/>
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="AE5" s="6">
         <f t="shared" si="20"/>
-        <v>0.56692913385826771</v>
+        <v>0.82677165354330706</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -1209,7 +1212,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="0"/>
@@ -1217,27 +1220,27 @@
       </c>
       <c r="K6" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20003108</v>
+        <v>0x20003140</v>
       </c>
       <c r="L6" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20003300</v>
+        <v>0x20003338</v>
       </c>
       <c r="M6" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20003180</v>
+        <v>0x200031b8</v>
       </c>
       <c r="N6" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20003108</v>
+        <v>20003140</v>
       </c>
       <c r="O6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003300</v>
+        <v>20003338</v>
       </c>
       <c r="P6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003180</v>
+        <v>200031b8</v>
       </c>
       <c r="Q6" s="3" t="str">
         <f t="shared" si="10"/>
@@ -1304,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1316,7 +1319,7 @@
         <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="0"/>
@@ -1324,39 +1327,39 @@
       </c>
       <c r="K7" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20003388</v>
+        <v>0x200033c0</v>
       </c>
       <c r="L7" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20003580</v>
+        <v>0x200035b8</v>
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20003458</v>
+        <v>0x20003488</v>
       </c>
       <c r="N7" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20003388</v>
+        <v>200033c0</v>
       </c>
       <c r="O7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003580</v>
+        <v>200035b8</v>
       </c>
       <c r="P7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003458</v>
+        <v>20003488</v>
       </c>
       <c r="Q7" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>296/504</v>
+        <v>304/504</v>
       </c>
       <c r="R7" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="S7" s="4">
         <f>INT(_xlfn.IFNA(LEFT(R7,LEN(R7)-1)*CHOOSE(MATCH(RIGHT(R7,1), {"K","M","B"},0),1000,1000000,1000000000),R7))</f>
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="T7" s="3" t="str">
         <f t="shared" si="2"/>
@@ -1380,11 +1383,11 @@
       </c>
       <c r="Z7" s="5">
         <f t="shared" si="15"/>
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="AA7" s="6">
         <f t="shared" si="16"/>
-        <v>0.41269841269841268</v>
+        <v>0.3968253968253968</v>
       </c>
       <c r="AB7" s="7">
         <f t="shared" si="17"/>
@@ -1392,15 +1395,15 @@
       </c>
       <c r="AC7" s="7">
         <f t="shared" si="18"/>
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="AD7" s="7">
         <f t="shared" si="19"/>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AE7" s="6">
         <f t="shared" si="20"/>
-        <v>0.58730158730158732</v>
+        <v>0.60317460317460314</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -1416,39 +1419,39 @@
       </c>
       <c r="K8" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20003608</v>
+        <v>0x20003640</v>
       </c>
       <c r="L8" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20003800</v>
+        <v>0x20003838</v>
       </c>
       <c r="M8" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x200036b0</v>
+        <v>0x20003710</v>
       </c>
       <c r="N8" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20003608</v>
+        <v>20003640</v>
       </c>
       <c r="O8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>20003800</v>
+        <v>20003838</v>
       </c>
       <c r="P8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>200036b0</v>
+        <v>20003710</v>
       </c>
       <c r="Q8" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>336/504</v>
+        <v>296/504</v>
       </c>
       <c r="R8" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>336</v>
+        <v>296</v>
       </c>
       <c r="S8" s="4">
         <f>INT(_xlfn.IFNA(LEFT(R8,LEN(R8)-1)*CHOOSE(MATCH(RIGHT(R8,1), {"K","M","B"},0),1000,1000000,1000000000),R8))</f>
-        <v>336</v>
+        <v>296</v>
       </c>
       <c r="T8" s="3" t="str">
         <f t="shared" si="2"/>
@@ -1472,11 +1475,11 @@
       </c>
       <c r="Z8" s="5">
         <f t="shared" si="15"/>
-        <v>168</v>
+        <v>208</v>
       </c>
       <c r="AA8" s="6">
         <f t="shared" si="16"/>
-        <v>0.33333333333333331</v>
+        <v>0.41269841269841268</v>
       </c>
       <c r="AB8" s="7">
         <f t="shared" si="17"/>
@@ -1484,15 +1487,15 @@
       </c>
       <c r="AC8" s="7">
         <f t="shared" si="18"/>
-        <v>336</v>
+        <v>296</v>
       </c>
       <c r="AD8" s="7">
         <f t="shared" si="19"/>
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="AE8" s="6">
         <f t="shared" si="20"/>
-        <v>0.66666666666666663</v>
+        <v>0.58730158730158732</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -1500,7 +1503,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" ref="J9:J35" si="21">MATCH(W9, $A:$A, 0)</f>
@@ -1508,27 +1511,27 @@
       </c>
       <c r="K9" s="3" t="str">
         <f t="shared" si="6"/>
-        <v>0x20003888</v>
+        <v>0x200038c0</v>
       </c>
       <c r="L9" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>0x20003980</v>
+        <v>0x200039b8</v>
       </c>
       <c r="M9" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>0x20003928</v>
+        <v>0x20003960</v>
       </c>
       <c r="N9" s="3" t="str">
         <f t="shared" ref="N9:N35" si="22">RIGHT(K9,LEN(K9)-2)</f>
-        <v>20003888</v>
+        <v>200038c0</v>
       </c>
       <c r="O9" s="3" t="str">
         <f t="shared" ref="O9:O35" si="23">RIGHT(L9,LEN(L9)-2)</f>
-        <v>20003980</v>
+        <v>200039b8</v>
       </c>
       <c r="P9" s="3" t="str">
         <f t="shared" ref="P9:P35" si="24">RIGHT(M9,LEN(M9)-2)</f>
-        <v>20003928</v>
+        <v>20003960</v>
       </c>
       <c r="Q9" s="3" t="str">
         <f t="shared" si="10"/>
@@ -1592,7 +1595,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="J10" s="5" t="e">
         <f t="shared" si="21"/>
@@ -1684,7 +1687,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J11" s="5" t="e">
         <f t="shared" si="21"/>
@@ -1779,7 +1782,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
@@ -1788,10 +1791,10 @@
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="J12" s="5" t="e">
         <f t="shared" si="21"/>
@@ -1975,7 +1978,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="J14" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2067,7 +2070,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J15" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2159,7 +2162,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J16" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2254,7 +2257,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -2263,10 +2266,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J17" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2450,7 +2453,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="J19" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2542,7 +2545,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="J20" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2634,7 +2637,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="J21" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2729,7 +2732,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -2741,7 +2744,7 @@
         <v>44</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J22" s="5" t="e">
         <f t="shared" si="21"/>
@@ -2925,7 +2928,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="J24" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3017,7 +3020,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J25" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3109,7 +3112,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="J26" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3201,10 +3204,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -3213,10 +3216,10 @@
         <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="J27" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3400,7 +3403,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="J29" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3492,7 +3495,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J30" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3584,7 +3587,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J31" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3679,19 +3682,19 @@
         <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J32" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3875,7 +3878,7 @@
         <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J34" s="5" t="e">
         <f t="shared" si="21"/>
@@ -3967,7 +3970,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J35" s="5" t="e">
         <f t="shared" si="21"/>
@@ -4059,7 +4062,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J36" s="9" t="e">
         <f t="shared" ref="J36:J99" si="36">MATCH(W36, $A:$A, 0)</f>
@@ -4154,7 +4157,7 @@
         <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>1</v>
@@ -4163,10 +4166,10 @@
         <v>25</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J37" s="9" t="e">
         <f t="shared" si="36"/>
@@ -4350,7 +4353,7 @@
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J39" s="9" t="e">
         <f t="shared" si="36"/>
@@ -4442,7 +4445,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J40" s="9" t="e">
         <f t="shared" si="36"/>
@@ -4534,7 +4537,7 @@
         <v>15</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J41" s="9" t="e">
         <f t="shared" si="36"/>

</xml_diff>